<commit_message>
Adding a bunch of things
</commit_message>
<xml_diff>
--- a/docs/Results.xlsx
+++ b/docs/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21105"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17560" tabRatio="500" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="BernoulliNB" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="38">
   <si>
     <t>Classifier</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>Difference between Preprocessing and No Preprocessing</t>
+  </si>
+  <si>
+    <t>P-Value</t>
   </si>
 </sst>
 </file>
@@ -645,13 +648,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="409">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1064,87 +1067,7 @@
     <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="76">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="68">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2176,108 +2099,108 @@
       <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13" t="s">
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13" t="s">
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13" t="s">
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13" t="s">
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13" t="s">
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
     </row>
     <row r="4" spans="1:18">
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13" t="s">
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13" t="s">
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13" t="s">
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
     </row>
     <row r="5" spans="1:18" s="3" customFormat="1" ht="33" customHeight="1">
       <c r="C5" s="3" t="s">
@@ -5997,6 +5920,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="O3:R3"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="C3:F3"/>
@@ -6005,14 +5936,6 @@
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="G3:J3"/>
     <mergeCell ref="G4:J4"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="O4:R4"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="O3:R3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6058,204 +5981,204 @@
       <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13" t="s">
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13" t="s">
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13" t="s">
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="14" t="s">
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="13" t="s">
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="13"/>
-      <c r="AE1" s="14" t="s">
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AF1" s="14"/>
-      <c r="AG1" s="14"/>
-      <c r="AH1" s="14"/>
+      <c r="AF1" s="15"/>
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15"/>
     </row>
     <row r="2" spans="1:34">
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13" t="s">
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13" t="s">
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="14" t="s">
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="13" t="s">
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="AB2" s="13"/>
-      <c r="AC2" s="13"/>
-      <c r="AD2" s="13"/>
-      <c r="AE2" s="14" t="s">
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="14"/>
+      <c r="AE2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="AF2" s="14"/>
-      <c r="AG2" s="14"/>
-      <c r="AH2" s="14"/>
+      <c r="AF2" s="15"/>
+      <c r="AG2" s="15"/>
+      <c r="AH2" s="15"/>
     </row>
     <row r="3" spans="1:34">
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13" t="s">
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13" t="s">
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13" t="s">
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13"/>
-      <c r="W3" s="14" t="s">
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="14"/>
-      <c r="AA3" s="13" t="s">
+      <c r="X3" s="15"/>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="15"/>
+      <c r="AA3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="AB3" s="13"/>
-      <c r="AC3" s="13"/>
-      <c r="AD3" s="13"/>
-      <c r="AE3" s="14" t="s">
+      <c r="AB3" s="14"/>
+      <c r="AC3" s="14"/>
+      <c r="AD3" s="14"/>
+      <c r="AE3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="AF3" s="14"/>
-      <c r="AG3" s="14"/>
-      <c r="AH3" s="14"/>
+      <c r="AF3" s="15"/>
+      <c r="AG3" s="15"/>
+      <c r="AH3" s="15"/>
     </row>
     <row r="4" spans="1:34">
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13" t="s">
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13" t="s">
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13" t="s">
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13" t="s">
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="13"/>
-      <c r="W4" s="14" t="s">
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="14"/>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="13" t="s">
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="AB4" s="13"/>
-      <c r="AC4" s="13"/>
-      <c r="AD4" s="13"/>
-      <c r="AE4" s="14" t="s">
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14"/>
+      <c r="AE4" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="AF4" s="14"/>
-      <c r="AG4" s="14"/>
-      <c r="AH4" s="14"/>
+      <c r="AF4" s="15"/>
+      <c r="AG4" s="15"/>
+      <c r="AH4" s="15"/>
     </row>
     <row r="5" spans="1:34" s="3" customFormat="1" ht="33" customHeight="1">
       <c r="C5" s="3" t="s">
@@ -13038,12 +12961,18 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="AE4:AH4"/>
+    <mergeCell ref="AE1:AH1"/>
+    <mergeCell ref="AA2:AD2"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AA3:AD3"/>
+    <mergeCell ref="AE3:AH3"/>
+    <mergeCell ref="W1:Z1"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="W3:Z3"/>
+    <mergeCell ref="W4:Z4"/>
+    <mergeCell ref="AA1:AD1"/>
+    <mergeCell ref="AA4:AD4"/>
     <mergeCell ref="S3:V3"/>
     <mergeCell ref="S4:V4"/>
     <mergeCell ref="C3:F3"/>
@@ -13054,22 +12983,16 @@
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="K4:N4"/>
     <mergeCell ref="O4:R4"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="S2:V2"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="O1:R1"/>
-    <mergeCell ref="W1:Z1"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="W3:Z3"/>
-    <mergeCell ref="W4:Z4"/>
-    <mergeCell ref="AA1:AD1"/>
-    <mergeCell ref="AA4:AD4"/>
-    <mergeCell ref="AE4:AH4"/>
-    <mergeCell ref="AE1:AH1"/>
-    <mergeCell ref="AA2:AD2"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AA3:AD3"/>
-    <mergeCell ref="AE3:AH3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -13107,114 +13030,114 @@
       <c r="B1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14" t="s">
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14" t="s">
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14" t="s">
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14" t="s">
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14" t="s">
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14" t="s">
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14" t="s">
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14" t="s">
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14" t="s">
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
     </row>
     <row r="5" spans="1:18" ht="45">
       <c r="A5" s="7"/>
@@ -16696,6 +16619,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="O4:R4"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="K1:N1"/>
@@ -16704,14 +16635,6 @@
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="O2:R2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="O4:R4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -16749,108 +16672,108 @@
       <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13" t="s">
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13" t="s">
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13" t="s">
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13" t="s">
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13" t="s">
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
     </row>
     <row r="4" spans="1:18">
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13" t="s">
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13" t="s">
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13" t="s">
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
     </row>
     <row r="5" spans="1:18" s="3" customFormat="1" ht="33" customHeight="1">
       <c r="C5" s="3" t="s">
@@ -20587,6 +20510,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="O4:R4"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="K1:N1"/>
@@ -20595,14 +20526,6 @@
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="O2:R2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="O4:R4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -20635,114 +20558,114 @@
       <c r="B1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14" t="s">
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14" t="s">
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14" t="s">
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14" t="s">
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14" t="s">
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14" t="s">
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14" t="s">
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14" t="s">
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14" t="s">
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
     </row>
     <row r="5" spans="1:18" ht="45">
       <c r="A5" s="7"/>
@@ -27061,6 +26984,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="O4:R4"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="K1:N1"/>
@@ -27069,14 +27000,6 @@
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="O2:R2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="O4:R4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -27103,114 +27026,114 @@
       <c r="B1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14" t="s">
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14" t="s">
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14" t="s">
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14" t="s">
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14" t="s">
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14" t="s">
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14" t="s">
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14" t="s">
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14" t="s">
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
     </row>
     <row r="5" spans="1:18" ht="45">
       <c r="A5" s="7"/>
@@ -30692,6 +30615,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="O4:R4"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="K1:N1"/>
@@ -30700,14 +30631,6 @@
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="O2:R2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="O4:R4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -30723,8 +30646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC53"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -31697,6 +31620,9 @@
       <c r="E29" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="F29" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="4" t="s">
@@ -31711,7 +31637,7 @@
       <c r="D30" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="13">
         <f>MultinomialNB!$H$6</f>
         <v>2.1964503636888198E-2</v>
       </c>
@@ -31733,7 +31659,7 @@
       <c r="D31" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E31" s="13">
         <f>MultinomialNB!$P$6</f>
         <v>2.1090408874156176E-2</v>
       </c>
@@ -31755,7 +31681,7 @@
       <c r="D32" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="13">
         <f>BernoulliNB!$H$6</f>
         <v>1.4416258001644623E-2</v>
       </c>
@@ -31777,7 +31703,7 @@
       <c r="D33" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E33" s="13">
         <f>BernoulliNB!$P$6</f>
         <v>1.4216591374115857E-2</v>
       </c>
@@ -31799,7 +31725,7 @@
       <c r="D34" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E34" s="13">
         <f>MultinomialNB!$L$6</f>
         <v>4.2746162963445749E-3</v>
       </c>
@@ -31821,7 +31747,7 @@
       <c r="D35" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E35" s="15">
+      <c r="E35" s="13">
         <f>BernoulliNB!$L$6</f>
         <v>4.1551128503735631E-3</v>
       </c>
@@ -31843,7 +31769,7 @@
       <c r="D36" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E36" s="15">
+      <c r="E36" s="13">
         <f>'KNN1000'!$H$6</f>
         <v>2.3106189161775439E-3</v>
       </c>
@@ -31865,7 +31791,7 @@
       <c r="D37" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E37" s="13">
         <f>'KNN2000'!$H$6</f>
         <v>1.828853622169459E-3</v>
       </c>
@@ -31887,7 +31813,7 @@
       <c r="D38" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="15">
+      <c r="E38" s="13">
         <f>MultinomialNB!$D$6</f>
         <v>1.6459023702842651E-3</v>
       </c>
@@ -31909,7 +31835,7 @@
       <c r="D39" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="15">
+      <c r="E39" s="13">
         <f>BernoulliNB!$D$6</f>
         <v>1.5627947902664607E-3</v>
       </c>
@@ -31931,7 +31857,7 @@
       <c r="D40" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E40" s="15">
+      <c r="E40" s="13">
         <f>'KNN1000'!$P$6</f>
         <v>1.2034464900695125E-3</v>
       </c>
@@ -31953,7 +31879,7 @@
       <c r="D41" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E41" s="15">
+      <c r="E41" s="13">
         <f>'KNN2000'!$P$6</f>
         <v>8.116978442044107E-4</v>
       </c>
@@ -31975,7 +31901,7 @@
       <c r="D42" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E42" s="15">
+      <c r="E42" s="13">
         <f>'KNN2000'!$L$6</f>
         <v>0</v>
       </c>
@@ -31997,7 +31923,7 @@
       <c r="D43" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E43" s="15">
+      <c r="E43" s="13">
         <f>'KNN2000'!$D$6</f>
         <v>-1.2251174066664935E-5</v>
       </c>
@@ -32019,7 +31945,7 @@
       <c r="D44" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E44" s="15">
+      <c r="E44" s="13">
         <f>'KNN1000'!$L$6</f>
         <v>-8.7801634117452702E-5</v>
       </c>
@@ -32041,7 +31967,7 @@
       <c r="D45" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E45" s="15">
+      <c r="E45" s="13">
         <f>'KNN1000'!$D$6</f>
         <v>-2.3817228363656647E-4</v>
       </c>
@@ -32063,7 +31989,7 @@
       <c r="D46" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E46" s="15">
+      <c r="E46" s="13">
         <f>'KNN100'!$H$6</f>
         <v>-1.5646684370040358E-3</v>
       </c>
@@ -32085,7 +32011,7 @@
       <c r="D47" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E47" s="15">
+      <c r="E47" s="13">
         <f>'KNN50'!$H$6</f>
         <v>-5.3408244306301176E-3</v>
       </c>
@@ -32107,7 +32033,7 @@
       <c r="D48" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E48" s="15">
+      <c r="E48" s="13">
         <f>'KNN100'!$P$6</f>
         <v>-7.8768309958076495E-3</v>
       </c>
@@ -32129,7 +32055,7 @@
       <c r="D49" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E49" s="15">
+      <c r="E49" s="13">
         <f>'KNN100'!$D$6</f>
         <v>-8.0884745188880506E-3</v>
       </c>
@@ -32151,7 +32077,7 @@
       <c r="D50" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E50" s="15">
+      <c r="E50" s="13">
         <f>'KNN100'!$L$6</f>
         <v>-8.8017534253455633E-3</v>
       </c>
@@ -32173,7 +32099,7 @@
       <c r="D51" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E51" s="15">
+      <c r="E51" s="13">
         <f>'KNN50'!$D$6</f>
         <v>-1.1730735070668663E-2</v>
       </c>
@@ -32195,7 +32121,7 @@
       <c r="D52" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E52" s="15">
+      <c r="E52" s="13">
         <f>'KNN50'!$P$6</f>
         <v>-1.180177827858709E-2</v>
       </c>
@@ -32217,7 +32143,7 @@
       <c r="D53" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="15">
+      <c r="E53" s="13">
         <f>'KNN50'!$L$6</f>
         <v>-1.2135117285782994E-2</v>
       </c>
@@ -32231,250 +32157,250 @@
     <sortCondition descending="1" ref="E30:E53"/>
   </sortState>
   <conditionalFormatting sqref="B8">
-    <cfRule type="cellIs" dxfId="71" priority="105" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="67" priority="105" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="106" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="66" priority="106" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:E8">
-    <cfRule type="cellIs" dxfId="69" priority="103" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="65" priority="103" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="104" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="104" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="cellIs" dxfId="67" priority="101" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="63" priority="101" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="102" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="102" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:E11">
-    <cfRule type="cellIs" dxfId="65" priority="99" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="61" priority="99" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="100" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="100" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="cellIs" dxfId="63" priority="97" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="59" priority="97" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="98" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="98" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:E14">
-    <cfRule type="cellIs" dxfId="61" priority="95" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="57" priority="95" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="96" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="56" priority="96" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="cellIs" dxfId="59" priority="93" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="55" priority="93" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="94" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="94" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:E17">
-    <cfRule type="cellIs" dxfId="57" priority="91" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="53" priority="91" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="92" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="52" priority="92" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="cellIs" dxfId="55" priority="89" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="51" priority="89" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="90" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="90" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:E20">
-    <cfRule type="cellIs" dxfId="53" priority="87" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="49" priority="87" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="88" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="88" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="51" priority="45" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="47" priority="45" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="46" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="46" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17:K17">
-    <cfRule type="cellIs" dxfId="49" priority="43" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="45" priority="43" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="44" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="44" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="47" priority="57" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="43" priority="57" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="58" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="58" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:K8">
-    <cfRule type="cellIs" dxfId="45" priority="55" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="41" priority="55" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="56" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="56" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="43" priority="53" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="39" priority="53" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="54" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="54" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:K11">
-    <cfRule type="cellIs" dxfId="41" priority="51" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="37" priority="51" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="52" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="52" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="cellIs" dxfId="39" priority="49" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="35" priority="49" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="50" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="50" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:K14">
-    <cfRule type="cellIs" dxfId="37" priority="47" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="33" priority="47" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="48" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="48" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N11">
-    <cfRule type="cellIs" dxfId="35" priority="33" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="31" priority="33" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="34" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="34" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O11:Q11">
-    <cfRule type="cellIs" dxfId="33" priority="31" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="29" priority="31" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="32" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N14">
-    <cfRule type="cellIs" dxfId="31" priority="29" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="27" priority="29" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="30" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O14:Q14">
-    <cfRule type="cellIs" dxfId="29" priority="27" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="28" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8">
-    <cfRule type="cellIs" dxfId="27" priority="37" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="23" priority="37" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="38" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O8:Q8">
-    <cfRule type="cellIs" dxfId="25" priority="35" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="21" priority="35" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="36" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T8">
-    <cfRule type="cellIs" dxfId="23" priority="21" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="22" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U8:W8">
-    <cfRule type="cellIs" dxfId="21" priority="19" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T11">
-    <cfRule type="cellIs" dxfId="19" priority="17" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U11:W11">
-    <cfRule type="cellIs" dxfId="17" priority="15" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z8">
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA8:AC8">
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:E53">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -35960,8 +35886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68:M68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>